<commit_message>
teacher services done correctly
</commit_message>
<xml_diff>
--- a/DB/TeacherDB.xlsx
+++ b/DB/TeacherDB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\SchoolSystem\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F859F5-226F-4103-9752-A738C7A5860D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F27DFAE-6832-4184-9D00-284EC0ACBEE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="180" yWindow="168" windowWidth="12036" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7080" yWindow="168" windowWidth="12036" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Teacher Details " sheetId="3" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>ID</t>
   </si>
@@ -52,7 +52,7 @@
     <t>1-&gt;English</t>
   </si>
   <si>
-    <t>Teacher1@</t>
+    <t>teacher1@gmail.com</t>
   </si>
   <si>
     <t>1 cairo street</t>
@@ -68,6 +68,30 @@
   </si>
   <si>
     <t>2 cairo street</t>
+  </si>
+  <si>
+    <t>teacher10</t>
+  </si>
+  <si>
+    <t>6-&gt;Arabic</t>
+  </si>
+  <si>
+    <t>teacher10@</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cairo street</t>
+  </si>
+  <si>
+    <t>1-&gt;histroy</t>
+  </si>
+  <si>
+    <t>teacher5@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">street </t>
+  </si>
+  <si>
+    <t>teacher5</t>
   </si>
 </sst>
 </file>
@@ -419,10 +443,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -461,13 +485,13 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
       </c>
       <c r="E2">
-        <v>11111111</v>
+        <v>1111111111</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -481,25 +505,25 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="C3">
         <v>35</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="E3">
-        <v>11111111</v>
+        <v>2222222222</v>
       </c>
       <c r="F3" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="H3" t="b">
         <v>0</v>
@@ -507,27 +531,53 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C4">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="E4">
-        <v>2222222</v>
+        <v>1010101010</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="H4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5">
+        <v>33</v>
+      </c>
+      <c r="D5" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5">
+        <v>2020202020</v>
+      </c>
+      <c r="F5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>